<commit_message>
made updates to figures
</commit_message>
<xml_diff>
--- a/final regression and uncertainties.xlsx
+++ b/final regression and uncertainties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerzeigler/Documents/Flowers Lab/Apatite Nano-CT Project_Feb 2019_June 2020/apatite-project-git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659E6AE2-667A-F54F-8BE2-E3CD874C9B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2BB84B-4CC6-6745-8DD8-5D20F58219FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-400" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{D5CDA270-30C0-964D-9D34-D59A27B36975}"/>
   </bookViews>
@@ -452,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DE5003-094F-7244-96B1-392C8F0415D2}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="262" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G6" zoomScale="284" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
post-color update on figures
</commit_message>
<xml_diff>
--- a/final regression and uncertainties.xlsx
+++ b/final regression and uncertainties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerzeigler/Documents/Flowers Lab/Apatite Nano-CT Project_Feb 2019_June 2020/apatite-project-git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2BB84B-4CC6-6745-8DD8-5D20F58219FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C63953-53F3-A64D-A161-617F7CA8C89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-400" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{D5CDA270-30C0-964D-9D34-D59A27B36975}"/>
+    <workbookView xWindow="39080" yWindow="-1140" windowWidth="28040" windowHeight="17440" xr2:uid="{D5CDA270-30C0-964D-9D34-D59A27B36975}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
   <si>
     <t>Hexagonal</t>
   </si>
@@ -91,6 +91,39 @@
   </si>
   <si>
     <t>category</t>
+  </si>
+  <si>
+    <t>Ft</t>
+  </si>
+  <si>
+    <t>Rs</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Hex Correction</t>
+  </si>
+  <si>
+    <t>Ellipsoid Correction</t>
+  </si>
+  <si>
+    <t>Uncertainty</t>
+  </si>
+  <si>
+    <t>Rough</t>
+  </si>
+  <si>
+    <t>Smooth</t>
   </si>
 </sst>
 </file>
@@ -450,288 +483,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1DE5003-094F-7244-96B1-392C8F0415D2}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G6" zoomScale="284" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="219" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1.0088159999999999</v>
+      </c>
+      <c r="C2">
+        <v>1.868212</v>
+      </c>
+      <c r="D2">
+        <v>4.4052550000000004</v>
+      </c>
+      <c r="E2">
+        <v>10.463767000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1.082856</v>
+      </c>
+      <c r="G2">
+        <v>5.045992</v>
+      </c>
+      <c r="Q2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="R2" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="H1" t="s">
+      <c r="V2" s="1"/>
+      <c r="X2" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="Y2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="Z2" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AA2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.0262450000000001</v>
+      </c>
+      <c r="C3">
+        <v>6.802238</v>
+      </c>
+      <c r="D3">
+        <v>7.0806570000000004</v>
+      </c>
+      <c r="E3">
+        <v>9.6264769999999995</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.1706570000000001</v>
+      </c>
+      <c r="G3">
+        <v>9.6937370000000005</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
-        <v>1.0088159999999999</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="T3" s="2">
         <v>2.661348E-3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="U3" s="2">
         <v>0.99155899999999997</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="H2" t="s">
+      <c r="V3" s="1"/>
+      <c r="X3" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
+      <c r="Y3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="Z3" t="s">
         <v>9</v>
       </c>
-      <c r="K2">
-        <v>10.463767000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Q4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
-        <v>1.082856</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="T4" s="2">
         <v>8.8797779999999996E-3</v>
       </c>
-      <c r="E3" s="2">
+      <c r="U4" s="2">
         <v>0.92348370000000002</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="H3" t="s">
+      <c r="V4" s="1"/>
+      <c r="X4" t="s">
         <v>8</v>
       </c>
-      <c r="I3" t="s">
+      <c r="Y4" t="s">
         <v>5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="Z4" t="s">
         <v>10</v>
       </c>
-      <c r="K3">
-        <v>4.4052550000000004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2">
+      <c r="T5" s="2">
+        <v>1.254738E-2</v>
+      </c>
+      <c r="U5" s="2">
+        <v>1.021844</v>
+      </c>
+      <c r="X5" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2">
         <v>0.97936570000000001</v>
       </c>
-      <c r="D4" s="2">
-        <v>1.254738E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.021844</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="C6">
+        <v>16.44162</v>
+      </c>
+      <c r="D6">
+        <v>23.9056</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.3393856</v>
+      </c>
+      <c r="G6">
+        <v>22.434004999999999</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T6" s="2">
+        <v>5.7032670000000001E-2</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0.74660839999999995</v>
+      </c>
+      <c r="X6" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Q7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T7" s="2">
+        <v>4.7395780000000004E-3</v>
+      </c>
+      <c r="U7" s="2">
+        <v>0.97489979999999998</v>
+      </c>
+      <c r="X7" t="s">
         <v>8</v>
       </c>
-      <c r="I4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="Y7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Q8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1.9622379999999998E-2</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.85422100000000001</v>
+      </c>
+      <c r="X8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="X9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="X10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="X11" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="X12" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z12" t="s">
         <v>11</v>
       </c>
-      <c r="K4">
-        <v>1.868212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="X13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2">
-        <v>1.3393856</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5.7032670000000001E-2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.74660839999999995</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="Y13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z13" t="s">
         <v>12</v>
-      </c>
-      <c r="K5">
-        <v>5.045992</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1.0262450000000001</v>
-      </c>
-      <c r="D6" s="2">
-        <v>4.7395780000000004E-3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.97489979999999998</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6">
-        <v>16.44162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1.1706570000000001</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1.9622379999999998E-2</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.85422100000000001</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K7">
-        <v>23.9056</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H8" t="s">
-        <v>4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" t="s">
-        <v>12</v>
-      </c>
-      <c r="K8">
-        <v>22.434004999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K9">
-        <v>9.6264769999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" t="s">
-        <v>7</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10">
-        <v>7.0806570000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H11" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" t="s">
-        <v>7</v>
-      </c>
-      <c r="J11" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11">
-        <v>6.802238</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I12" t="s">
-        <v>7</v>
-      </c>
-      <c r="J12" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12">
-        <v>9.6937370000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>